<commit_message>
InvoiceDate to datetime and initial churn rate exploration.
</commit_message>
<xml_diff>
--- a/Project_plan_CP_v23_09_22.xlsx
+++ b/Project_plan_CP_v23_09_22.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b37d5b112f2106df/Documents/Study/SUPSI/Year 3/data_challenge_3/admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data challenge 3\project_1\data_challenge_3_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B20E59A3-DAD0-402E-AA87-46CEB9573623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4273E2-DF8C-4A06-AE15-EA3D2A3C0159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="3852" windowWidth="17280" windowHeight="9420" xr2:uid="{7A7D0F82-19BC-4D4C-8900-8B53D9DA9A08}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" xr2:uid="{7A7D0F82-19BC-4D4C-8900-8B53D9DA9A08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,7 +621,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C9" sqref="C5:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tuned model and results reporting.
Cluster analysis for the NLP side of the project.
</commit_message>
<xml_diff>
--- a/Project_plan_CP_v23_09_22.xlsx
+++ b/Project_plan_CP_v23_09_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data challenge 3\project_1\data_challenge_3_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB73A99-66C6-4E30-8C8E-B5E89CAC04FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F04F40-8085-47DB-A7D2-63D6C96D26E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{7A7D0F82-19BC-4D4C-8900-8B53D9DA9A08}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>W1</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>CB: preprocessing of partial cancelled orders, feature engineering, CP: basic model, defining twin customers</t>
+  </si>
+  <si>
+    <t>CB: time series CP: finish NLP, tune base model</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,7 +691,9 @@
       <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">

</xml_diff>